<commit_message>
Downweighted priors based on HF studies
</commit_message>
<xml_diff>
--- a/data-01_empirical-priors.xlsx
+++ b/data-01_empirical-priors.xlsx
@@ -384,7 +384,7 @@
         <v>-0.7019510651752735</v>
       </c>
       <c r="C2">
-        <v>0.2223047157779202</v>
+        <v>0.3143863440326309</v>
       </c>
     </row>
     <row r="3">
@@ -397,7 +397,7 @@
         <v>-0.7632790043340278</v>
       </c>
       <c r="C3">
-        <v>0.2205605095247896</v>
+        <v>0.3119196638938777</v>
       </c>
     </row>
     <row r="4">

</xml_diff>